<commit_message>
feat: automatic Git update on excel change
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arman\Desktop\parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E938E0F8-12B1-4694-BF26-6983C7535986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688595F8-8C70-469C-8AA2-99DA88CEB56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7170" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Название товара</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>бут</t>
+  </si>
+  <si>
+    <t>Teos</t>
   </si>
 </sst>
 </file>
@@ -435,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,21 +460,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -482,10 +485,10 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -496,10 +499,10 @@
         <v>9</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -513,7 +516,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -525,12 +528,26 @@
       </c>
       <c r="D6">
         <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>400</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:D1 A6:C6 A5:D5 A4:C4 A3:D3 A2 C2:D2" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:D1 B6:C6 A5:D5 A4:C4 A3:C3 A2 C2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>